<commit_message>
other CR and other comp box addition(lots of bugs in this one)
</commit_message>
<xml_diff>
--- a/MockData.xlsx
+++ b/MockData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB\Documents\R\Client-Elevator-App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89221E4F-DA56-471C-9E73-29961469E6F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B944059-5E0D-4BB5-B843-7598FE597E06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Client" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4119" uniqueCount="1000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4121" uniqueCount="1002">
   <si>
     <t>ID_Client</t>
   </si>
@@ -3024,6 +3024,12 @@
   </si>
   <si>
     <t>780 BOYLSTON-2</t>
+  </si>
+  <si>
+    <t>OtherComp</t>
+  </si>
+  <si>
+    <t>OtherCR</t>
   </si>
 </sst>
 </file>
@@ -3436,22 +3442,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O364"/>
+  <dimension ref="A1:Q364"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3497,8 +3515,14 @@
       <c r="O1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -3530,7 +3554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -3577,7 +3601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -3624,7 +3648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -3671,7 +3695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -3718,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -3765,7 +3789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -3812,7 +3836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -3859,7 +3883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -3906,7 +3930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -3953,7 +3977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -4000,7 +4024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -4047,7 +4071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -4094,7 +4118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -4141,7 +4165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -21570,8 +21594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>